<commit_message>
Just before demultiplexer overhaul
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/unige/desalt_plexed/metadata_plexed.xlsx
+++ b/metadata/excel/projects/unige/desalt_plexed/metadata_plexed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="40780" windowHeight="12640" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="920" windowWidth="40780" windowHeight="12640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_exp1_plexed" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
   <si>
     <t>Country</t>
   </si>
@@ -339,15 +339,9 @@
     <t>Optional extra data</t>
   </si>
   <si>
-    <t>Header barcode</t>
-  </si>
-  <si>
     <t>Multiplex group reference</t>
   </si>
   <si>
-    <t>Header rev. comp.</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -409,6 +403,24 @@
   </si>
   <si>
     <t>Single run of the V1V2 desalt project plexed</t>
+  </si>
+  <si>
+    <t>v1v2_plexed</t>
+  </si>
+  <si>
+    <t>V1V2</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>GCTTGTCTCAAAGATTAAGCC</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>CCTGCTGCCTTCCTTRGA</t>
   </si>
 </sst>
 </file>
@@ -419,7 +431,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -551,6 +563,14 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -916,7 +936,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1048,6 +1068,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="290"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="291">
     <cellStyle name="Excel Built-in Normal" xfId="267"/>
@@ -1731,12 +1754,12 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:CD31"/>
+  <dimension ref="A1:CA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="117" zoomScaleNormal="117" zoomScalePageLayoutView="117" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="117" zoomScaleNormal="117" zoomScalePageLayoutView="117" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomLeft" activeCell="AR11" sqref="AR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1753,76 +1776,72 @@
     <col min="10" max="10" width="29.83203125" style="36" customWidth="1"/>
     <col min="11" max="11" width="23" style="35" customWidth="1"/>
     <col min="12" max="12" width="31.1640625" style="35" customWidth="1"/>
-    <col min="13" max="13" width="32.6640625" style="35" customWidth="1"/>
-    <col min="14" max="14" width="11.5" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" style="35" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="35" customWidth="1"/>
-    <col min="17" max="17" width="30.33203125" style="31" customWidth="1"/>
-    <col min="18" max="18" width="11.5" customWidth="1"/>
-    <col min="19" max="19" width="15.83203125" style="54" customWidth="1"/>
-    <col min="20" max="20" width="14" style="57" customWidth="1"/>
-    <col min="21" max="22" width="16.83203125" customWidth="1"/>
-    <col min="23" max="23" width="11.5" customWidth="1"/>
-    <col min="24" max="24" width="43.6640625" style="19" customWidth="1"/>
-    <col min="25" max="25" width="44.33203125" style="19" customWidth="1"/>
-    <col min="26" max="26" width="9.83203125" customWidth="1"/>
-    <col min="27" max="27" width="25.5" style="45" customWidth="1"/>
-    <col min="28" max="28" width="20.1640625" style="19" customWidth="1"/>
-    <col min="29" max="29" width="22" style="22" customWidth="1"/>
-    <col min="30" max="30" width="17.83203125" style="45" customWidth="1"/>
-    <col min="31" max="31" width="21.5" style="19" customWidth="1"/>
-    <col min="32" max="32" width="27.6640625" style="23" customWidth="1"/>
-    <col min="33" max="33" width="9.83203125" customWidth="1"/>
-    <col min="34" max="34" width="11" customWidth="1"/>
-    <col min="35" max="35" width="13.5" style="2" customWidth="1"/>
-    <col min="36" max="36" width="9.1640625" customWidth="1"/>
-    <col min="37" max="37" width="14.33203125" style="2" customWidth="1"/>
-    <col min="38" max="38" width="15.83203125" style="2" customWidth="1"/>
-    <col min="39" max="39" width="8.5" customWidth="1"/>
-    <col min="40" max="40" width="10.33203125" style="17" customWidth="1"/>
-    <col min="41" max="41" width="10.33203125" customWidth="1"/>
-    <col min="42" max="42" width="11.5" customWidth="1"/>
-    <col min="43" max="43" width="19.6640625" customWidth="1"/>
-    <col min="44" max="44" width="12.83203125" style="58" customWidth="1"/>
-    <col min="45" max="45" width="32.83203125" style="1" customWidth="1"/>
-    <col min="46" max="46" width="13" style="58" customWidth="1"/>
-    <col min="47" max="47" width="35.6640625" style="1" customWidth="1"/>
-    <col min="48" max="48" width="10.1640625" customWidth="1"/>
-    <col min="49" max="49" width="12.5" customWidth="1"/>
-    <col min="50" max="50" width="15" customWidth="1"/>
-    <col min="51" max="51" width="10.83203125" customWidth="1"/>
-    <col min="52" max="52" width="14" customWidth="1"/>
-    <col min="53" max="53" width="13.1640625" customWidth="1"/>
-    <col min="54" max="54" width="15.6640625" customWidth="1"/>
-    <col min="55" max="55" width="11.6640625" customWidth="1"/>
-    <col min="56" max="56" width="12.1640625" customWidth="1"/>
-    <col min="57" max="57" width="13" customWidth="1"/>
-    <col min="58" max="58" width="10.1640625" customWidth="1"/>
-    <col min="59" max="61" width="19.83203125" customWidth="1"/>
-    <col min="62" max="62" width="20.83203125" customWidth="1"/>
-    <col min="63" max="63" width="8.6640625" customWidth="1"/>
-    <col min="64" max="64" width="15.5" customWidth="1"/>
-    <col min="65" max="65" width="13.6640625" style="12" customWidth="1"/>
-    <col min="66" max="66" width="13.1640625" style="12" customWidth="1"/>
-    <col min="67" max="67" width="12.5" style="19" customWidth="1"/>
-    <col min="68" max="68" width="26" style="19" customWidth="1"/>
-    <col min="69" max="69" width="31.33203125" style="19" customWidth="1"/>
-    <col min="70" max="70" width="9" customWidth="1"/>
-    <col min="71" max="71" width="16.5" customWidth="1"/>
-    <col min="72" max="72" width="16" customWidth="1"/>
-    <col min="73" max="73" width="9.5" customWidth="1"/>
-    <col min="74" max="74" width="11" style="25" customWidth="1"/>
-    <col min="75" max="75" width="11.6640625" style="25" customWidth="1"/>
-    <col min="76" max="76" width="14.33203125" style="25" customWidth="1"/>
-    <col min="77" max="77" width="12.6640625" style="25" customWidth="1"/>
-    <col min="78" max="78" width="13.6640625" style="25" customWidth="1"/>
-    <col min="79" max="79" width="15.33203125" style="25" customWidth="1"/>
-    <col min="80" max="80" width="15.5" style="25" customWidth="1"/>
-    <col min="81" max="81" width="14.6640625" style="25" customWidth="1"/>
-    <col min="82" max="82" width="9.6640625" customWidth="1"/>
+    <col min="13" max="14" width="32.6640625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" style="54" customWidth="1"/>
+    <col min="17" max="17" width="14" style="57" customWidth="1"/>
+    <col min="18" max="19" width="16.83203125" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="43.6640625" style="19" customWidth="1"/>
+    <col min="22" max="22" width="44.33203125" style="19" customWidth="1"/>
+    <col min="23" max="23" width="9.83203125" customWidth="1"/>
+    <col min="24" max="24" width="25.5" style="45" customWidth="1"/>
+    <col min="25" max="25" width="20.1640625" style="19" customWidth="1"/>
+    <col min="26" max="26" width="22" style="22" customWidth="1"/>
+    <col min="27" max="27" width="17.83203125" style="45" customWidth="1"/>
+    <col min="28" max="28" width="21.5" style="19" customWidth="1"/>
+    <col min="29" max="29" width="27.6640625" style="23" customWidth="1"/>
+    <col min="30" max="30" width="9.83203125" customWidth="1"/>
+    <col min="31" max="31" width="11" customWidth="1"/>
+    <col min="32" max="32" width="13.5" style="2" customWidth="1"/>
+    <col min="33" max="33" width="9.1640625" customWidth="1"/>
+    <col min="34" max="34" width="14.33203125" style="2" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="8.5" customWidth="1"/>
+    <col min="37" max="37" width="10.33203125" style="17" customWidth="1"/>
+    <col min="38" max="38" width="10.33203125" customWidth="1"/>
+    <col min="39" max="39" width="11.5" customWidth="1"/>
+    <col min="40" max="40" width="19.6640625" customWidth="1"/>
+    <col min="41" max="41" width="12.83203125" style="58" customWidth="1"/>
+    <col min="42" max="42" width="32.83203125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="13" style="58" customWidth="1"/>
+    <col min="44" max="44" width="35.6640625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="10.1640625" customWidth="1"/>
+    <col min="46" max="46" width="12.5" customWidth="1"/>
+    <col min="47" max="47" width="15" customWidth="1"/>
+    <col min="48" max="48" width="10.83203125" customWidth="1"/>
+    <col min="49" max="49" width="14" customWidth="1"/>
+    <col min="50" max="50" width="13.1640625" customWidth="1"/>
+    <col min="51" max="51" width="15.6640625" customWidth="1"/>
+    <col min="52" max="52" width="11.6640625" customWidth="1"/>
+    <col min="53" max="53" width="12.1640625" customWidth="1"/>
+    <col min="54" max="54" width="13" customWidth="1"/>
+    <col min="55" max="55" width="10.1640625" customWidth="1"/>
+    <col min="56" max="58" width="19.83203125" customWidth="1"/>
+    <col min="59" max="59" width="20.83203125" customWidth="1"/>
+    <col min="60" max="60" width="8.6640625" customWidth="1"/>
+    <col min="61" max="61" width="15.5" customWidth="1"/>
+    <col min="62" max="62" width="13.6640625" style="12" customWidth="1"/>
+    <col min="63" max="63" width="13.1640625" style="12" customWidth="1"/>
+    <col min="64" max="64" width="12.5" style="19" customWidth="1"/>
+    <col min="65" max="65" width="26" style="19" customWidth="1"/>
+    <col min="66" max="66" width="31.33203125" style="19" customWidth="1"/>
+    <col min="67" max="67" width="9" customWidth="1"/>
+    <col min="68" max="68" width="16.5" customWidth="1"/>
+    <col min="69" max="69" width="16" customWidth="1"/>
+    <col min="70" max="70" width="9.5" customWidth="1"/>
+    <col min="71" max="71" width="11" style="25" customWidth="1"/>
+    <col min="72" max="72" width="11.6640625" style="25" customWidth="1"/>
+    <col min="73" max="73" width="14.33203125" style="25" customWidth="1"/>
+    <col min="74" max="74" width="12.6640625" style="25" customWidth="1"/>
+    <col min="75" max="75" width="13.6640625" style="25" customWidth="1"/>
+    <col min="76" max="76" width="15.33203125" style="25" customWidth="1"/>
+    <col min="77" max="77" width="15.5" style="25" customWidth="1"/>
+    <col min="78" max="78" width="14.6640625" style="25" customWidth="1"/>
+    <col min="79" max="79" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -1836,74 +1855,72 @@
       <c r="K1" s="33"/>
       <c r="L1" s="33"/>
       <c r="M1" s="34"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="47"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="7"/>
-      <c r="X1" s="7"/>
+      <c r="N1" s="34"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="20"/>
+      <c r="X1" s="44"/>
       <c r="Y1" s="20"/>
-      <c r="AA1" s="44"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="46"/>
       <c r="AB1" s="20"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="6"/>
       <c r="AI1" s="6"/>
       <c r="AJ1" s="4"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="4"/>
-      <c r="AQ1" s="9"/>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="8"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="4"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="8"/>
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="4"/>
+      <c r="AV1" s="4"/>
       <c r="AW1" s="4"/>
       <c r="AX1" s="4"/>
       <c r="AY1" s="4"/>
       <c r="AZ1" s="4"/>
       <c r="BA1" s="4"/>
-      <c r="BB1" s="4"/>
-      <c r="BC1" s="4"/>
-      <c r="BD1" s="4"/>
-      <c r="BE1" s="11"/>
-      <c r="BG1" s="59" t="s">
+      <c r="BB1" s="11"/>
+      <c r="BD1" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="BH1" s="59"/>
-      <c r="BI1" s="59"/>
+      <c r="BE1" s="59"/>
+      <c r="BF1" s="59"/>
+      <c r="BG1" s="59"/>
+      <c r="BI1" s="59" t="s">
+        <v>52</v>
+      </c>
       <c r="BJ1" s="59"/>
-      <c r="BL1" s="59" t="s">
-        <v>52</v>
-      </c>
+      <c r="BK1" s="59"/>
+      <c r="BL1" s="59"/>
       <c r="BM1" s="59"/>
       <c r="BN1" s="59"/>
-      <c r="BO1" s="59"/>
-      <c r="BP1" s="59"/>
+      <c r="BP1" s="59" t="s">
+        <v>66</v>
+      </c>
       <c r="BQ1" s="59"/>
-      <c r="BS1" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT1" s="59"/>
-      <c r="BV1" s="9" t="s">
+      <c r="BS1" s="9" t="s">
         <v>71</v>
       </c>
+      <c r="BT1" s="24"/>
+      <c r="BU1" s="24"/>
+      <c r="BV1" s="24"/>
       <c r="BW1" s="24"/>
       <c r="BX1" s="24"/>
       <c r="BY1" s="24"/>
       <c r="BZ1" s="24"/>
-      <c r="CA1" s="24"/>
-      <c r="CB1" s="24"/>
-      <c r="CC1" s="24"/>
-    </row>
-    <row r="2" spans="1:82" s="43" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:79" s="43" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>49</v>
       </c>
@@ -1911,7 +1928,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>65</v>
@@ -1922,7 +1939,7 @@
       <c r="F2" s="48"/>
       <c r="G2" s="48"/>
       <c r="H2" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I2" s="37" t="s">
         <v>61</v>
@@ -1939,390 +1956,401 @@
       <c r="M2" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="49"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="P2" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q2" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2" s="49"/>
-      <c r="S2" s="52" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="52" t="s">
+      <c r="Q2" s="52" t="s">
         <v>58</v>
       </c>
+      <c r="R2" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="49"/>
       <c r="U2" s="37" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="V2" s="37" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="W2" s="49"/>
       <c r="X2" s="37" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="Y2" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z2" s="49"/>
+        <v>16</v>
+      </c>
+      <c r="Z2" s="37" t="s">
+        <v>17</v>
+      </c>
       <c r="AA2" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AB2" s="37" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AC2" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD2" s="37" t="s">
-        <v>54</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="AD2" s="49"/>
       <c r="AE2" s="37" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="AF2" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG2" s="49"/>
+        <v>45</v>
+      </c>
+      <c r="AG2" s="37" t="s">
+        <v>43</v>
+      </c>
       <c r="AH2" s="37" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AI2" s="37" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AJ2" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK2" s="37" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="AK2" s="38" t="s">
+        <v>39</v>
       </c>
       <c r="AL2" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM2" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="AN2" s="38" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="37" t="s">
+        <v>1</v>
       </c>
       <c r="AO2" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP2" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="AP2" s="37" t="s">
+        <v>3</v>
+      </c>
       <c r="AQ2" s="37" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AR2" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS2" s="37" t="s">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="AS2" s="50"/>
       <c r="AT2" s="37" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="AU2" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="AV2" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="AV2" s="37" t="s">
+        <v>22</v>
+      </c>
       <c r="AW2" s="37" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AX2" s="37" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AY2" s="37" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="AZ2" s="37" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="BA2" s="37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="BB2" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="BC2" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="BD2" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="BE2" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="BF2" s="50"/>
+      <c r="BC2" s="50"/>
+      <c r="BD2" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="BE2" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="BF2" s="39" t="s">
+        <v>34</v>
+      </c>
       <c r="BG2" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="BH2" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="BI2" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="BJ2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="BK2" s="50"/>
+      <c r="BH2" s="50"/>
+      <c r="BI2" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ2" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK2" s="40" t="s">
+        <v>13</v>
+      </c>
       <c r="BL2" s="40" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="BM2" s="40" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="BN2" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="BO2" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="BP2" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="BQ2" s="40" t="s">
         <v>36</v>
       </c>
+      <c r="BO2" s="50"/>
+      <c r="BP2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ2" s="41" t="s">
+        <v>7</v>
+      </c>
       <c r="BR2" s="50"/>
-      <c r="BS2" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="BT2" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="BU2" s="50"/>
+      <c r="BS2" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="BT2" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="BU2" s="42" t="s">
+        <v>42</v>
+      </c>
       <c r="BV2" s="42" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="BW2" s="42" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="BX2" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BY2" s="42" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="BZ2" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="CA2" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="CB2" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="CC2" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="CD2" s="50"/>
-    </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="CA2" s="50"/>
+    </row>
+    <row r="3" spans="1:79" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
-        <f t="shared" ref="A3" si="0">COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BQ3,"&lt;&gt;"&amp;"")</f>
+        <f>COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BN3,"&lt;&gt;"&amp;"")</f>
         <v>1</v>
       </c>
       <c r="B3" s="26">
         <v>1</v>
       </c>
       <c r="C3" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="I3" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="36" t="s">
+      <c r="P3" s="53">
+        <v>7349733</v>
+      </c>
+      <c r="Q3" s="56">
+        <v>7349733</v>
+      </c>
+      <c r="R3" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="T3" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="K3" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="L3" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="M3" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="S3" s="53">
-        <v>7349733</v>
-      </c>
-      <c r="T3" s="56">
-        <v>7349733</v>
-      </c>
-      <c r="U3" s="29" t="s">
+      <c r="V3" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="Y3" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA3" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB3" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC3" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="19" t="s">
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="14"/>
+      <c r="AN3" t="s">
         <v>95</v>
       </c>
-      <c r="Y3" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AO3" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AQ3" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS3" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB3" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC3" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD3" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE3" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF3" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL3" s="18"/>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="16"/>
-      <c r="AO3" s="14"/>
+      <c r="AT3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>9</v>
+      </c>
       <c r="AV3" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="AW3" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="AX3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>67</v>
-      </c>
-      <c r="BA3" t="s">
         <v>11</v>
       </c>
-      <c r="BL3" s="27"/>
-      <c r="BM3" s="28"/>
+      <c r="BI3" s="27"/>
+      <c r="BJ3" s="28"/>
+      <c r="BK3" s="28"/>
+      <c r="BL3"/>
+      <c r="BM3"/>
       <c r="BN3" s="28"/>
-      <c r="BO3"/>
-      <c r="BP3"/>
-      <c r="BQ3" s="28"/>
+      <c r="BS3"/>
+      <c r="BT3"/>
+      <c r="BU3"/>
       <c r="BV3"/>
       <c r="BW3"/>
       <c r="BX3"/>
       <c r="BY3"/>
       <c r="BZ3"/>
-      <c r="CA3"/>
-      <c r="CB3"/>
-      <c r="CC3"/>
-    </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO4" s="14"/>
-    </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO5" s="14"/>
-    </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO6" s="14"/>
-    </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO7" s="14"/>
-    </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO8" s="14"/>
-    </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO9" s="14"/>
-    </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO10" s="14"/>
-    </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO11" s="14"/>
-    </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO12" s="14"/>
-    </row>
-    <row r="13" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO13" s="14"/>
-    </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO14" s="14"/>
-    </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO15" s="14"/>
-    </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.2">
-      <c r="AO16" s="14"/>
-    </row>
-    <row r="17" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO17" s="14"/>
-    </row>
-    <row r="18" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO18" s="14"/>
-    </row>
-    <row r="19" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO19" s="14"/>
-    </row>
-    <row r="20" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO20" s="14"/>
-    </row>
-    <row r="21" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO21" s="14"/>
-    </row>
-    <row r="22" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO22" s="14"/>
-    </row>
-    <row r="23" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO23" s="14"/>
-    </row>
-    <row r="24" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO24" s="14"/>
-    </row>
-    <row r="25" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO25" s="14"/>
-    </row>
-    <row r="26" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO26" s="14"/>
-    </row>
-    <row r="27" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO27" s="14"/>
-    </row>
-    <row r="28" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO28" s="14"/>
-    </row>
-    <row r="29" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO29" s="14"/>
-    </row>
-    <row r="30" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO30" s="14"/>
-    </row>
-    <row r="31" spans="41:41" x14ac:dyDescent="0.2">
-      <c r="AO31" s="14"/>
+    </row>
+    <row r="4" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL4" s="14"/>
+    </row>
+    <row r="5" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL5" s="14"/>
+    </row>
+    <row r="6" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL6" s="14"/>
+    </row>
+    <row r="7" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL7" s="14"/>
+    </row>
+    <row r="8" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL8" s="14"/>
+    </row>
+    <row r="9" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL9" s="14"/>
+    </row>
+    <row r="10" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL10" s="14"/>
+    </row>
+    <row r="11" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL11" s="14"/>
+    </row>
+    <row r="12" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL12" s="14"/>
+    </row>
+    <row r="13" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL13" s="14"/>
+    </row>
+    <row r="14" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL14" s="14"/>
+    </row>
+    <row r="15" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL15" s="14"/>
+    </row>
+    <row r="16" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AL16" s="14"/>
+    </row>
+    <row r="17" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL17" s="14"/>
+    </row>
+    <row r="18" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL18" s="14"/>
+    </row>
+    <row r="19" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL19" s="14"/>
+    </row>
+    <row r="20" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL20" s="14"/>
+    </row>
+    <row r="21" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL21" s="14"/>
+    </row>
+    <row r="22" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL22" s="14"/>
+    </row>
+    <row r="23" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL23" s="14"/>
+    </row>
+    <row r="24" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL24" s="14"/>
+    </row>
+    <row r="25" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL25" s="14"/>
+    </row>
+    <row r="26" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL26" s="14"/>
+    </row>
+    <row r="27" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL27" s="14"/>
+    </row>
+    <row r="28" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL28" s="14"/>
+    </row>
+    <row r="29" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL29" s="14"/>
+    </row>
+    <row r="30" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL30" s="14"/>
+    </row>
+    <row r="31" spans="38:38" x14ac:dyDescent="0.2">
+      <c r="AL31" s="14"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -2368,30 +2396,30 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
-    <mergeCell ref="BG1:BJ1"/>
-    <mergeCell ref="BL1:BQ1"/>
-    <mergeCell ref="BS1:BT1"/>
+    <mergeCell ref="BD1:BG1"/>
+    <mergeCell ref="BI1:BN1"/>
+    <mergeCell ref="BP1:BQ1"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="AN3">
+  <conditionalFormatting sqref="AK3">
     <cfRule type="containsBlanks" dxfId="4" priority="9" stopIfTrue="1">
-      <formula>LEN(TRIM(AN3))=0</formula>
+      <formula>LEN(TRIM(AK3))=0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
       <formula>0.02</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:T3">
+  <conditionalFormatting sqref="P3:Q3">
     <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
       <formula>2000</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="7">
-      <formula>$S3&lt;&gt;$T3</formula>
+      <formula>$P3&lt;&gt;$Q3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:T1048576">
+  <conditionalFormatting sqref="P2:Q1048576">
     <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>LEN(TRIM(S2))=0</formula>
+      <formula>LEN(TRIM(P2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A1048576">
@@ -2404,7 +2432,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AC3" r:id="rId1"/>
+    <hyperlink ref="Z3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>